<commit_message>
Added new column Fertilizer used per area to the master dataset
</commit_message>
<xml_diff>
--- a/Correlation_data.xlsx
+++ b/Correlation_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R15"/>
+  <dimension ref="A1:S15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -491,35 +491,40 @@
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
+          <t>Fertilizer Use Per Area</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
           <t>Fertilizer Use Per Capita</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Credit to Agriculture</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>FDI inflows to Agriculture</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>Agriculture share of Government Expenditure</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>Water Use Efficiency</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>Gini coefficient</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>Agri_Prod_Per_Capita</t>
         </is>
@@ -562,24 +567,27 @@
         <v>-0.02</v>
       </c>
       <c r="L2" t="n">
+        <v>-0.5600000000000001</v>
+      </c>
+      <c r="M2" t="n">
         <v>-0.54</v>
       </c>
-      <c r="M2" t="n">
+      <c r="N2" t="n">
         <v>-0.4</v>
-      </c>
-      <c r="N2" t="n">
-        <v>0.09</v>
       </c>
       <c r="O2" t="n">
         <v>0.09</v>
       </c>
       <c r="P2" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="Q2" t="n">
         <v>-0.73</v>
       </c>
-      <c r="Q2" t="n">
+      <c r="R2" t="n">
         <v>-0</v>
       </c>
-      <c r="R2" t="n">
+      <c r="S2" t="n">
         <v>1</v>
       </c>
     </row>
@@ -620,20 +628,23 @@
         <v>0.28</v>
       </c>
       <c r="L3" t="n">
+        <v>-0.1</v>
+      </c>
+      <c r="M3" t="n">
         <v>-0.05</v>
       </c>
-      <c r="M3" t="inlineStr"/>
       <c r="N3" t="inlineStr"/>
-      <c r="O3" t="n">
+      <c r="O3" t="inlineStr"/>
+      <c r="P3" t="n">
         <v>0.45</v>
       </c>
-      <c r="P3" t="n">
+      <c r="Q3" t="n">
         <v>-0.16</v>
       </c>
-      <c r="Q3" t="n">
+      <c r="R3" t="n">
         <v>0.44</v>
       </c>
-      <c r="R3" t="n">
+      <c r="S3" t="n">
         <v>1</v>
       </c>
     </row>
@@ -674,22 +685,25 @@
         <v>0.9399999999999999</v>
       </c>
       <c r="L4" t="n">
+        <v>-0.45</v>
+      </c>
+      <c r="M4" t="n">
         <v>0.5600000000000001</v>
       </c>
-      <c r="M4" t="inlineStr"/>
-      <c r="N4" t="n">
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="n">
         <v>0.07000000000000001</v>
       </c>
-      <c r="O4" t="n">
+      <c r="P4" t="n">
         <v>0.3</v>
       </c>
-      <c r="P4" t="n">
+      <c r="Q4" t="n">
         <v>-0.47</v>
       </c>
-      <c r="Q4" t="n">
+      <c r="R4" t="n">
         <v>0.93</v>
       </c>
-      <c r="R4" t="n">
+      <c r="S4" t="n">
         <v>1</v>
       </c>
     </row>
@@ -730,20 +744,23 @@
         <v>0.88</v>
       </c>
       <c r="L5" t="n">
+        <v>0.67</v>
+      </c>
+      <c r="M5" t="n">
         <v>0.53</v>
       </c>
-      <c r="M5" t="inlineStr"/>
-      <c r="N5" t="n">
+      <c r="N5" t="inlineStr"/>
+      <c r="O5" t="n">
         <v>-0.35</v>
       </c>
-      <c r="O5" t="n">
+      <c r="P5" t="n">
         <v>-0.26</v>
       </c>
-      <c r="P5" t="n">
+      <c r="Q5" t="n">
         <v>-0.45</v>
       </c>
-      <c r="Q5" t="inlineStr"/>
-      <c r="R5" t="n">
+      <c r="R5" t="inlineStr"/>
+      <c r="S5" t="n">
         <v>1</v>
       </c>
     </row>
@@ -782,22 +799,25 @@
         <v>0.6899999999999999</v>
       </c>
       <c r="L6" t="n">
+        <v>-0.58</v>
+      </c>
+      <c r="M6" t="n">
         <v>-0.6</v>
       </c>
-      <c r="M6" t="inlineStr"/>
-      <c r="N6" t="n">
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" t="n">
         <v>0.3</v>
       </c>
-      <c r="O6" t="n">
+      <c r="P6" t="n">
         <v>-0.53</v>
       </c>
-      <c r="P6" t="n">
+      <c r="Q6" t="n">
         <v>0.79</v>
       </c>
-      <c r="Q6" t="n">
+      <c r="R6" t="n">
         <v>0.65</v>
       </c>
-      <c r="R6" t="n">
+      <c r="S6" t="n">
         <v>1</v>
       </c>
     </row>
@@ -838,22 +858,25 @@
         <v>0.82</v>
       </c>
       <c r="L7" t="n">
+        <v>-0.22</v>
+      </c>
+      <c r="M7" t="n">
         <v>-0.63</v>
       </c>
-      <c r="M7" t="inlineStr"/>
-      <c r="N7" t="n">
+      <c r="N7" t="inlineStr"/>
+      <c r="O7" t="n">
         <v>0.3</v>
       </c>
-      <c r="O7" t="n">
+      <c r="P7" t="n">
         <v>-0.65</v>
       </c>
-      <c r="P7" t="n">
+      <c r="Q7" t="n">
         <v>-0.23</v>
       </c>
-      <c r="Q7" t="n">
+      <c r="R7" t="n">
         <v>-0.08</v>
       </c>
-      <c r="R7" t="n">
+      <c r="S7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -894,22 +917,25 @@
         <v>0.44</v>
       </c>
       <c r="L8" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="M8" t="n">
         <v>-0.23</v>
       </c>
-      <c r="M8" t="n">
+      <c r="N8" t="n">
         <v>0.26</v>
       </c>
-      <c r="N8" t="inlineStr"/>
-      <c r="O8" t="n">
+      <c r="O8" t="inlineStr"/>
+      <c r="P8" t="n">
         <v>-0.4</v>
       </c>
-      <c r="P8" t="n">
+      <c r="Q8" t="n">
         <v>-0.35</v>
       </c>
-      <c r="Q8" t="n">
+      <c r="R8" t="n">
         <v>-0.1</v>
       </c>
-      <c r="R8" t="n">
+      <c r="S8" t="n">
         <v>1</v>
       </c>
     </row>
@@ -950,24 +976,27 @@
         <v>0.77</v>
       </c>
       <c r="L9" t="n">
+        <v>0.8100000000000001</v>
+      </c>
+      <c r="M9" t="n">
         <v>0.92</v>
       </c>
-      <c r="M9" t="n">
+      <c r="N9" t="n">
         <v>0.72</v>
       </c>
-      <c r="N9" t="n">
+      <c r="O9" t="n">
         <v>0.33</v>
       </c>
-      <c r="O9" t="n">
+      <c r="P9" t="n">
         <v>-0.76</v>
       </c>
-      <c r="P9" t="n">
+      <c r="Q9" t="n">
         <v>0.74</v>
       </c>
-      <c r="Q9" t="n">
+      <c r="R9" t="n">
         <v>-0.86</v>
       </c>
-      <c r="R9" t="n">
+      <c r="S9" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1006,24 +1035,27 @@
         <v>0.88</v>
       </c>
       <c r="L10" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="M10" t="n">
         <v>-0.75</v>
       </c>
-      <c r="M10" t="n">
+      <c r="N10" t="n">
         <v>0.9</v>
       </c>
-      <c r="N10" t="n">
+      <c r="O10" t="n">
         <v>-0.07000000000000001</v>
       </c>
-      <c r="O10" t="n">
+      <c r="P10" t="n">
         <v>0.1</v>
       </c>
-      <c r="P10" t="n">
+      <c r="Q10" t="n">
         <v>0.5</v>
       </c>
-      <c r="Q10" t="n">
+      <c r="R10" t="n">
         <v>0.77</v>
       </c>
-      <c r="R10" t="n">
+      <c r="S10" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1050,6 +1082,7 @@
       <c r="P11" t="inlineStr"/>
       <c r="Q11" t="inlineStr"/>
       <c r="R11" t="inlineStr"/>
+      <c r="S11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1088,22 +1121,25 @@
         <v>0.24</v>
       </c>
       <c r="L12" t="n">
+        <v>-0.07000000000000001</v>
+      </c>
+      <c r="M12" t="n">
         <v>-0.08</v>
       </c>
-      <c r="M12" t="inlineStr"/>
-      <c r="N12" t="n">
+      <c r="N12" t="inlineStr"/>
+      <c r="O12" t="n">
         <v>-0.06</v>
       </c>
-      <c r="O12" t="n">
+      <c r="P12" t="n">
         <v>-0.19</v>
       </c>
-      <c r="P12" t="n">
+      <c r="Q12" t="n">
         <v>0.26</v>
       </c>
-      <c r="Q12" t="n">
+      <c r="R12" t="n">
         <v>-0.68</v>
       </c>
-      <c r="R12" t="n">
+      <c r="S12" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1130,6 +1166,7 @@
       <c r="P13" t="inlineStr"/>
       <c r="Q13" t="inlineStr"/>
       <c r="R13" t="inlineStr"/>
+      <c r="S13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1154,6 +1191,7 @@
       <c r="P14" t="inlineStr"/>
       <c r="Q14" t="inlineStr"/>
       <c r="R14" t="inlineStr"/>
+      <c r="S14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1192,22 +1230,25 @@
         <v>-0.83</v>
       </c>
       <c r="L15" t="n">
+        <v>0.66</v>
+      </c>
+      <c r="M15" t="n">
         <v>0.68</v>
       </c>
-      <c r="M15" t="inlineStr"/>
-      <c r="N15" t="n">
+      <c r="N15" t="inlineStr"/>
+      <c r="O15" t="n">
         <v>0.8100000000000001</v>
       </c>
-      <c r="O15" t="n">
+      <c r="P15" t="n">
         <v>0.66</v>
       </c>
-      <c r="P15" t="n">
+      <c r="Q15" t="n">
         <v>-0.76</v>
       </c>
-      <c r="Q15" t="n">
+      <c r="R15" t="n">
         <v>-0.03</v>
       </c>
-      <c r="R15" t="n">
+      <c r="S15" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>